<commit_message>
Add BOM things and PNs
</commit_message>
<xml_diff>
--- a/BOMs/sinking-clock-BOM-v3.xlsx
+++ b/BOMs/sinking-clock-BOM-v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507D5346-1D7F-44FF-8D30-FAE4AFBCCE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD710EC-6600-497C-8945-D4603B7A75D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain PCB Assembly" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="320">
   <si>
     <t>Quantity</t>
   </si>
@@ -601,21 +601,6 @@
     <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/4149/10123800</t>
   </si>
   <si>
-    <t>STM32</t>
-  </si>
-  <si>
-    <t>pull-up resistors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connector - Male Receptacle </t>
-  </si>
-  <si>
-    <t>buttons</t>
-  </si>
-  <si>
-    <t>buzzer</t>
-  </si>
-  <si>
     <t>battery</t>
   </si>
   <si>
@@ -922,21 +907,12 @@
     <t>https://www.digikey.com/en/products/detail/e-switch/TL3301DF160QG/1805555</t>
   </si>
   <si>
-    <t>Pin of Nails Connector</t>
-  </si>
-  <si>
     <t>Barrel Jack Connector</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/cui-devices/PJ-002BH-SMT-TR/404626</t>
   </si>
   <si>
-    <t>res</t>
-  </si>
-  <si>
-    <t>cap</t>
-  </si>
-  <si>
     <t>ferrite bead</t>
   </si>
   <si>
@@ -944,6 +920,84 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/ecs-inc/ECS-327-12-5-12R-TR/8593595</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>STM32G0 MCU</t>
+  </si>
+  <si>
+    <t>32-LQFP</t>
+  </si>
+  <si>
+    <t>STM32G031K8T6</t>
+  </si>
+  <si>
+    <t>497-19554-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/STM32G031K8T6/10300267</t>
+  </si>
+  <si>
+    <t>Resistor - 0 ohm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor - 10k ohm </t>
+  </si>
+  <si>
+    <t>Resistor - 56 ohm</t>
+  </si>
+  <si>
+    <t>0402</t>
+  </si>
+  <si>
+    <t>Capacitor - 4.7 uF</t>
+  </si>
+  <si>
+    <t>Capacitor - 12.5 pF</t>
+  </si>
+  <si>
+    <t>Capacitor - 100 nF</t>
+  </si>
+  <si>
+    <t>Capacitor - 100pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB Connector - Male Receptacle </t>
+  </si>
+  <si>
+    <t>SPDT Tactile Push Button Switch</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>DC Magnetic Buzzer</t>
+  </si>
+  <si>
+    <t>Plug of Nails SWD Connector</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>Tag-Connect</t>
+  </si>
+  <si>
+    <t>TC2030-IDC-NL</t>
+  </si>
+  <si>
+    <t>Capacitor - 10 uF</t>
+  </si>
+  <si>
+    <t>NMOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Green LEDs </t>
+  </si>
+  <si>
+    <t>DMN63D8L</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1179,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1193,6 +1247,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1482,29 +1545,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535EBE7C-EB1B-4F48-8827-B2C8DF8DD54E}">
-  <dimension ref="A1:L104"/>
+  <dimension ref="A1:M111"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="37.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="35.109375" customWidth="1"/>
-    <col min="7" max="7" width="9" style="11" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="13"/>
-    <col min="9" max="9" width="12.109375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="35.5546875" customWidth="1"/>
-    <col min="12" max="12" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="35.109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="9" style="11" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="13"/>
+    <col min="10" max="10" width="12.109375" style="13" customWidth="1"/>
+    <col min="11" max="11" width="35.5546875" customWidth="1"/>
+    <col min="13" max="13" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>45</v>
       </c>
@@ -1516,763 +1580,933 @@
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
       <c r="I1" s="29"/>
-    </row>
-    <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="29"/>
+    </row>
+    <row r="2" spans="1:13" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
       <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="10" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13">
+        <v>3.05</v>
+      </c>
+      <c r="J3" s="14">
+        <f t="shared" ref="J3:J75" si="0">H3*I3</f>
+        <v>3.05</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="M3" s="2">
+        <f>SUM(J3:J112)</f>
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>304</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>306</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>305</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>307</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>308</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="H12" s="11">
+        <v>1</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0.68</v>
+      </c>
+      <c r="J12" s="14">
+        <f t="shared" ref="J12" si="1">H12*I12</f>
+        <v>0.68</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>309</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="11">
+        <v>1</v>
+      </c>
+      <c r="I14" s="13">
+        <v>1.43</v>
+      </c>
+      <c r="J14" s="14">
+        <f t="shared" si="0"/>
+        <v>1.43</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>187</v>
       </c>
-      <c r="I3" s="14">
-        <f t="shared" ref="I3:I68" si="0">G3*H3</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="L3" s="2">
-        <f>SUM(I3:I105)</f>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>188</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>189</v>
+      </c>
+      <c r="J17" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>190</v>
+      </c>
+      <c r="J18" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>317</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="11">
+        <v>1</v>
+      </c>
+      <c r="I20" s="14">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>188</v>
-      </c>
-      <c r="I4" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>189</v>
-      </c>
-      <c r="I5" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>190</v>
-      </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>191</v>
-      </c>
-      <c r="I7" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>192</v>
-      </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>193</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>194</v>
-      </c>
-      <c r="I10" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>195</v>
-      </c>
-      <c r="I11" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>294</v>
-      </c>
-      <c r="I12" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>112</v>
-      </c>
-      <c r="G13" s="11">
-        <v>1</v>
-      </c>
-      <c r="H13" s="14">
+      <c r="J20" s="14">
+        <f>H20*I20</f>
         <v>0.24</v>
       </c>
-      <c r="I13" s="14">
-        <f>G13*H13</f>
-        <v>0.24</v>
-      </c>
-      <c r="J13" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>295</v>
-      </c>
-      <c r="I14" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>297</v>
-      </c>
-      <c r="I15" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>298</v>
-      </c>
-      <c r="I16" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>299</v>
-      </c>
-      <c r="I17" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>300</v>
-      </c>
-      <c r="I18" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I19" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I20" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I21" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I22" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I23" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I24" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I25" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I26" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I27" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I28" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I29" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I30" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I31" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I32" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I33" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I34" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I35" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I36" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I37" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I38" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I39" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I40" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I41" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I42" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I43" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I44" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I45" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I46" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I47" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I48" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I49" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I50" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I51" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I52" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I53" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I54" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I55" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I56" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I57" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I58" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I59" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I60" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I61" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I62" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I63" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I64" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I65" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I66" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I67" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I68" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I69" s="14">
-        <f t="shared" ref="I69:I104" si="1">G69*H69</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I70" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I71" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I72" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I73" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I74" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I75" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I76" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I77" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I78" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I79" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I80" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I81" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I82" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I83" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I84" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I85" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I86" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I87" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I88" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I89" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I90" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I91" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I92" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I93" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I94" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I95" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I96" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I97" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I98" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I99" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I100" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I101" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I102" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I103" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I104" s="14">
-        <f t="shared" si="1"/>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>289</v>
+      </c>
+      <c r="J21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>318</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="J22" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J23" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>291</v>
+      </c>
+      <c r="J24" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>292</v>
+      </c>
+      <c r="J25" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J26" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J27" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>312</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="J28" s="14">
+        <f>H28*I28</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J29" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J30" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J31" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J32" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J33" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J34" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J35" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J36" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J37" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J38" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J39" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J40" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J41" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J42" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J43" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J44" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J45" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J46" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J47" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J48" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J49" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J50" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J51" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J52" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J53" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J54" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J55" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J56" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J57" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J58" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J59" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J60" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J61" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J62" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J63" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J64" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J65" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J66" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J67" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J68" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J69" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J70" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J71" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J72" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J73" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J74" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J75" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J76" s="14">
+        <f t="shared" ref="J76:J111" si="2">H76*I76</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J77" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J78" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J79" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J80" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J81" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J82" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J83" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J84" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J85" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J86" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J87" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J88" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J89" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J90" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J91" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J92" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J93" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J94" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J95" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J96" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J97" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J98" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J99" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J100" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J101" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J102" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J103" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J104" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J105" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J106" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J107" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J108" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J109" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J110" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J111" s="14">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="K14" r:id="rId1" xr:uid="{206B78D0-3E11-49C8-918E-265464AE26FD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2282,7 +2516,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2346,19 +2580,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>57</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G3" s="11">
         <v>56</v>
@@ -2371,7 +2605,7 @@
         <v>7.9519999999999991</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="L3" s="2">
         <f>SUM(I3:I111)</f>
@@ -2380,19 +2614,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>57</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G4" s="11">
         <v>2</v>
@@ -2405,24 +2639,24 @@
         <v>0.4</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G5" s="11">
         <v>1</v>
@@ -2435,24 +2669,24 @@
         <v>0.32</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G6" s="11">
         <v>4</v>
@@ -2465,24 +2699,24 @@
         <v>1.88</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>227</v>
-      </c>
       <c r="D7" s="11" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="G7" s="11">
         <v>4</v>
@@ -2495,24 +2729,24 @@
         <v>0.4</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="G8" s="11">
         <v>1</v>
@@ -2525,24 +2759,24 @@
         <v>0.68</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G9" s="11">
         <v>1</v>
@@ -2555,24 +2789,24 @@
         <v>0.37</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="G10" s="11">
         <v>23</v>
@@ -2585,25 +2819,25 @@
         <v>4.4160000000000004</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G11" s="11">
         <v>3</v>
@@ -2616,24 +2850,24 @@
         <v>0.36</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G12" s="11">
         <v>4</v>
@@ -2646,24 +2880,24 @@
         <v>0.4</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G13" s="11">
         <v>5</v>
@@ -2676,24 +2910,24 @@
         <v>0.5</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G14" s="11">
         <v>12</v>
@@ -2706,24 +2940,24 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G15" s="11">
         <v>11</v>
@@ -2736,24 +2970,24 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C16" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>251</v>
-      </c>
       <c r="E16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G16" s="11">
         <v>2</v>
@@ -2766,24 +3000,24 @@
         <v>0.2</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G17" s="11">
         <v>9</v>
@@ -2796,7 +3030,7 @@
         <v>1.44</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
@@ -5725,8 +5959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B494BF-8FB3-4F10-BF9B-C1AB6CBBBD39}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -5793,22 +6027,22 @@
     </row>
     <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>57</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G3" s="20">
         <v>168</v>
@@ -5821,7 +6055,7 @@
         <v>23.855999999999998</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="L3" s="2">
         <f>SUM(I3:I101)</f>
@@ -5830,19 +6064,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>57</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G4" s="20">
         <v>6</v>
@@ -5855,24 +6089,24 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G5" s="20">
         <v>3</v>
@@ -5885,24 +6119,24 @@
         <v>0.96</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="19" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G6" s="20">
         <v>12</v>
@@ -5915,24 +6149,24 @@
         <v>5.64</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>227</v>
-      </c>
       <c r="D7" s="20" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="G7" s="20">
         <v>12</v>
@@ -5945,25 +6179,25 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="G8" s="20">
         <v>3</v>
@@ -5976,24 +6210,24 @@
         <v>2.04</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G9" s="20">
         <v>3</v>
@@ -6006,24 +6240,24 @@
         <v>1.1099999999999999</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="G10" s="20">
         <v>69</v>
@@ -6036,24 +6270,24 @@
         <v>13.248000000000001</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G11" s="20">
         <v>9</v>
@@ -6066,24 +6300,24 @@
         <v>1.08</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G12" s="20">
         <v>12</v>
@@ -6096,24 +6330,24 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G13" s="20">
         <v>15</v>
@@ -6126,24 +6360,24 @@
         <v>1.5</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G14" s="20">
         <v>36</v>
@@ -6156,24 +6390,24 @@
         <v>3.6</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" s="19" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G15" s="20">
         <v>33</v>
@@ -6186,24 +6420,24 @@
         <v>3.3000000000000003</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C16" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>251</v>
-      </c>
       <c r="E16" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G16" s="20">
         <v>4</v>
@@ -6216,24 +6450,24 @@
         <v>0.4</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="19" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G17" s="20">
         <v>27</v>
@@ -6246,24 +6480,24 @@
         <v>4.32</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="G18" s="11">
         <v>1</v>
@@ -6276,24 +6510,24 @@
         <v>22.16</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="G19" s="11">
         <v>1</v>
@@ -6306,24 +6540,24 @@
         <v>42.86</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>83</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G20" s="11">
         <v>1</v>
@@ -6336,21 +6570,21 @@
         <v>20.95</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F21" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="G21" s="11">
         <v>2</v>
@@ -6363,21 +6597,21 @@
         <v>0.42</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F22" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="G22" s="11">
         <v>2</v>
@@ -6390,21 +6624,21 @@
         <v>0.86</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F23" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="G23" s="11">
         <v>2</v>
@@ -6417,21 +6651,21 @@
         <v>0.86</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F24" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="G24" s="11">
         <v>2</v>
@@ -6444,7 +6678,7 @@
         <v>0.92</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add parameter changes to library, parameter instances to schematic doc, and outjob file
</commit_message>
<xml_diff>
--- a/BOMs/sinking-clock-BOM-v3.xlsx
+++ b/BOMs/sinking-clock-BOM-v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD710EC-6600-497C-8945-D4603B7A75D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8716F48C-F9B0-4F95-AAD3-CDB31C8ADD13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="330">
   <si>
     <t>Quantity</t>
   </si>
@@ -955,9 +955,6 @@
     <t>Capacitor - 4.7 uF</t>
   </si>
   <si>
-    <t>Capacitor - 12.5 pF</t>
-  </si>
-  <si>
     <t>Capacitor - 100 nF</t>
   </si>
   <si>
@@ -997,7 +994,40 @@
     <t xml:space="preserve">Green LEDs </t>
   </si>
   <si>
-    <t>DMN63D8L</t>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0402JR-0710KL/726418?s=N4IgTCBcDaIEoGEAMAWJYBScC0SDsAjEgNIAyIAugL5A</t>
+  </si>
+  <si>
+    <t>RC0402FR-070RL</t>
+  </si>
+  <si>
+    <t>CL05A475KQ5NRNC</t>
+  </si>
+  <si>
+    <t>CL05A104KP5NNNC</t>
+  </si>
+  <si>
+    <t>Capacitor - 7 pF</t>
+  </si>
+  <si>
+    <t>GJM1555C1H7R0DB01D</t>
+  </si>
+  <si>
+    <t>HH15N101J500CT</t>
+  </si>
+  <si>
+    <t>1292-HH15N101J500CT-ND</t>
+  </si>
+  <si>
+    <t>TSOT-23-6</t>
+  </si>
+  <si>
+    <t>2-SMD No Lead</t>
+  </si>
+  <si>
+    <t>ECS-.327-7-12R-TR</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
   </si>
 </sst>
 </file>
@@ -1236,6 +1266,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1247,15 +1286,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1549,15 +1579,15 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="37.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="33" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" style="11" customWidth="1"/>
     <col min="5" max="5" width="25.88671875" style="11" customWidth="1"/>
     <col min="6" max="6" width="16.77734375" style="11" customWidth="1"/>
     <col min="7" max="7" width="35.109375" style="11" customWidth="1"/>
@@ -1569,25 +1599,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:13" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
       <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="28" t="s">
         <v>294</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -1622,7 +1652,7 @@
       <c r="B3" t="s">
         <v>295</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="29" t="s">
         <v>296</v>
       </c>
       <c r="D3" s="11" t="s">
@@ -1659,8 +1689,17 @@
       <c r="B4" t="s">
         <v>300</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="30" t="s">
         <v>303</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="J4" s="14">
         <f t="shared" si="0"/>
@@ -1672,87 +1711,177 @@
       <c r="B5" t="s">
         <v>301</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>303</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>241</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="4"/>
+      <c r="F5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>302</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="30" t="s">
         <v>303</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>241</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="4"/>
+      <c r="F6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>316</v>
-      </c>
-      <c r="C7" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>303</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="4"/>
+      <c r="F7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>304</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="30" t="s">
         <v>303</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="D8" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>306</v>
-      </c>
-      <c r="C9" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>303</v>
       </c>
-      <c r="J9" s="14"/>
+      <c r="D9" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>305</v>
-      </c>
-      <c r="C10" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="C10" s="30" t="s">
         <v>303</v>
       </c>
-      <c r="J10" s="14"/>
+      <c r="D10" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>307</v>
-      </c>
-      <c r="C11" s="34" t="s">
+        <v>306</v>
+      </c>
+      <c r="C11" s="30" t="s">
         <v>303</v>
       </c>
-      <c r="J11" s="14"/>
+      <c r="D11" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>308</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>313</v>
+        <v>307</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>312</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>254</v>
@@ -1773,7 +1902,7 @@
         <v>0.68</v>
       </c>
       <c r="J12" s="14">
-        <f t="shared" ref="J12" si="1">H12*I12</f>
+        <f t="shared" si="0"/>
         <v>0.68</v>
       </c>
       <c r="K12" s="4" t="s">
@@ -1782,7 +1911,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="14">
@@ -1793,10 +1922,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>311</v>
-      </c>
-      <c r="C14" s="33" t="s">
         <v>310</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>309</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>72</v>
@@ -1826,118 +1955,151 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>187</v>
-      </c>
-      <c r="I15" s="14"/>
+        <v>292</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>328</v>
+      </c>
       <c r="J15" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="M15" s="2"/>
+      <c r="K15" s="4" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>188</v>
-      </c>
-      <c r="I16" s="14"/>
+        <v>316</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>225</v>
+      </c>
       <c r="J16" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>189</v>
+        <v>109</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" s="11">
+        <v>1</v>
+      </c>
+      <c r="I17" s="14">
+        <v>0.24</v>
       </c>
       <c r="J17" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+        <v>0.24</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>190</v>
+        <v>289</v>
       </c>
       <c r="J18" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K18" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>317</v>
       </c>
+      <c r="C19" s="29">
+        <v>603</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>202</v>
+      </c>
       <c r="E19" s="11" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="J19" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>109</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="H20" s="11">
-        <v>1</v>
-      </c>
-      <c r="I20" s="14">
-        <v>0.24</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="I20" s="14"/>
       <c r="J20" s="14">
-        <f>H20*I20</f>
-        <v>0.24</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>289</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="I21" s="14"/>
       <c r="J21" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K21" s="4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>318</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="J22" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>190</v>
+      </c>
       <c r="J23" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>291</v>
       </c>
@@ -1947,76 +2109,71 @@
       </c>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>292</v>
-      </c>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="J25" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K25" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="J26" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="J27" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
+        <v>311</v>
+      </c>
+      <c r="C28" s="29" t="s">
         <v>312</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="D28" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="E28" s="11" t="s">
         <v>314</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>315</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>266</v>
       </c>
       <c r="J28" s="14">
-        <f>H28*I28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="J29" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="J30" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="J31" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="J32" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2283,217 +2440,217 @@
     </row>
     <row r="76" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J76" s="14">
-        <f t="shared" ref="J76:J111" si="2">H76*I76</f>
+        <f t="shared" ref="J76:J111" si="1">H76*I76</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J77" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J78" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J79" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J80" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J81" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J82" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J83" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J84" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J85" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J86" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J87" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J88" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J89" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J90" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J91" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J92" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J93" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J94" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J95" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J96" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J97" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J98" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J99" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J100" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J101" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J102" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J103" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J104" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J105" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J106" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J107" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J108" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J109" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J110" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J111" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2504,9 +2661,10 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1" xr:uid="{206B78D0-3E11-49C8-918E-265464AE26FD}"/>
+    <hyperlink ref="K7" r:id="rId2" xr:uid="{6C5F0919-5E89-4DE3-A40D-FFBA722F20C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2535,15 +2693,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="A1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:12" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16"/>
@@ -3644,17 +3802,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
@@ -4827,17 +4985,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>
@@ -5980,17 +6138,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15"/>

</xml_diff>

<commit_message>
Add new master proj. Switch microcontroller.
</commit_message>
<xml_diff>
--- a/BOMs/sinking-clock-BOM-v3.xlsx
+++ b/BOMs/sinking-clock-BOM-v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE96C51-C451-439E-851B-C5A84C88D989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C73737-518C-4520-9073-8F6DFFD3204B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain PCB Assembly" sheetId="6" r:id="rId1"/>
@@ -928,18 +928,6 @@
     <t>STM32G0 MCU</t>
   </si>
   <si>
-    <t>32-LQFP</t>
-  </si>
-  <si>
-    <t>STM32G031K8T6</t>
-  </si>
-  <si>
-    <t>497-19554-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/STM32G031K8T6/10300267</t>
-  </si>
-  <si>
     <t>Resistor - 0 ohm</t>
   </si>
   <si>
@@ -1034,6 +1022,18 @@
   </si>
   <si>
     <t>Walsin Technology Corporation</t>
+  </si>
+  <si>
+    <t>48-LQFP</t>
+  </si>
+  <si>
+    <t>STM32G031C6T6</t>
+  </si>
+  <si>
+    <t>497-19555-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/STM32G031C6T6/10300268</t>
   </si>
 </sst>
 </file>
@@ -1584,8 +1584,8 @@
   <dimension ref="A1:M112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1659,50 +1659,50 @@
         <v>295</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>296</v>
+        <v>328</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>297</v>
+        <v>329</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>298</v>
+        <v>330</v>
       </c>
       <c r="H3" s="11">
         <v>1</v>
       </c>
       <c r="I3" s="13">
-        <v>3.05</v>
+        <v>3.31</v>
       </c>
       <c r="J3" s="14">
         <f t="shared" ref="J3:J76" si="0">H3*I3</f>
-        <v>3.05</v>
+        <v>3.31</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>299</v>
+        <v>331</v>
       </c>
       <c r="M3" s="2">
         <f>SUM(J3:J113)</f>
-        <v>5.4</v>
+        <v>5.66</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>241</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>12</v>
@@ -1715,10 +1715,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>241</v>
@@ -1737,15 +1737,15 @@
         <v>0</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>241</v>
@@ -1769,10 +1769,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>64</v>
@@ -1796,16 +1796,16 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>233</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>12</v>
@@ -1818,16 +1818,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>233</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>12</v>
@@ -1840,16 +1840,16 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>12</v>
@@ -1862,16 +1862,16 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>12</v>
@@ -1884,10 +1884,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>254</v>
@@ -1917,10 +1917,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="14">
@@ -1931,10 +1931,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>72</v>
@@ -1967,13 +1967,13 @@
         <v>292</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="J15" s="14">
         <f t="shared" si="0"/>
@@ -1985,10 +1985,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>226</v>
@@ -2006,7 +2006,7 @@
         <v>109</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>110</v>
@@ -2039,7 +2039,7 @@
         <v>289</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="J18" s="14">
         <f t="shared" si="0"/>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C19" s="29">
         <v>603</v>
@@ -2070,10 +2070,10 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>250</v>
@@ -2160,16 +2160,16 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>266</v>

</xml_diff>

<commit_message>
Brain PCB nearing completion - needs button and JST connector footprints
</commit_message>
<xml_diff>
--- a/BOMs/sinking-clock-BOM-v3.xlsx
+++ b/BOMs/sinking-clock-BOM-v3.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C73737-518C-4520-9073-8F6DFFD3204B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E436CD14-C5C1-4224-B61B-CBD52D2EE7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain PCB Assembly" sheetId="6" r:id="rId1"/>
     <sheet name="LED PCB Assembly" sheetId="5" r:id="rId2"/>
-    <sheet name="PR-1" sheetId="1" r:id="rId3"/>
-    <sheet name="PR-2" sheetId="3" r:id="rId4"/>
-    <sheet name="PR-3" sheetId="8" r:id="rId5"/>
+    <sheet name="Cable Assemblies" sheetId="10" r:id="rId3"/>
+    <sheet name="PR-1" sheetId="1" r:id="rId4"/>
+    <sheet name="PR-2" sheetId="3" r:id="rId5"/>
+    <sheet name="PR-3" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="337">
   <si>
     <t>Quantity</t>
   </si>
@@ -1034,6 +1035,21 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/stmicroelectronics/STM32G031C6T6/10300268</t>
+  </si>
+  <si>
+    <t>Barrel Jack-to-Plug, 2.5mm ID, 5" length</t>
+  </si>
+  <si>
+    <t>NTE Electronics, Inc</t>
+  </si>
+  <si>
+    <t>57-PRP2</t>
+  </si>
+  <si>
+    <t>2368-57-PRP2-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nte-electronics-inc/57-PRP2/11644414</t>
   </si>
 </sst>
 </file>
@@ -1583,9 +1599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535EBE7C-EB1B-4F48-8827-B2C8DF8DD54E}">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2081,7 +2097,10 @@
       <c r="E20" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="J20" s="14"/>
+      <c r="J20" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
@@ -2702,7 +2721,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8:J8"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3806,6 +3825,819 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7A9FC6-1251-4D6C-A8F0-29659EBD6918}">
+  <dimension ref="A1:L112"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="37.109375" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="35.109375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="9" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="13"/>
+    <col min="9" max="9" width="12.109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="35.5546875" customWidth="1"/>
+    <col min="12" max="12" width="18.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+    </row>
+    <row r="2" spans="1:12" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15"/>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="G3" s="11">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I3" s="14">
+        <f t="shared" ref="I3:I76" si="0">G3*H3</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="L3" s="2">
+        <f>SUM(I3:I113)</f>
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I4" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I5" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I6" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I7" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I8" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I9" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I10" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I11" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I12" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H13" s="14"/>
+      <c r="I13" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I14" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I15" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I16" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H17" s="14"/>
+      <c r="I17" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I18" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I19" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I20" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H21" s="14"/>
+      <c r="I21" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H22" s="14"/>
+      <c r="I22" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I23" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I24" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I25" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I26" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I27" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I28" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>306</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="I29" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I30" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I31" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="I32" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I33" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I34" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I35" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I36" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I37" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I38" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I39" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I40" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I41" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I42" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I43" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I44" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I45" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I46" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I47" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="9:10" x14ac:dyDescent="0.3">
+      <c r="I48" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I49" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I50" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I51" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I52" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I53" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I54" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I55" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I56" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I57" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I58" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I59" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I60" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I61" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I62" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I63" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I64" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I65" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I66" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I67" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I68" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I69" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I70" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I71" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I72" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I73" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I74" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I75" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I76" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I77" s="14">
+        <f t="shared" ref="I77:I112" si="1">G77*H77</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I78" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I79" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I80" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I81" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I82" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I83" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I84" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I85" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I86" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I87" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I88" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I89" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I90" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I91" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I92" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I93" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I94" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I95" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I96" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I97" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I98" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I99" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I100" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I101" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I102" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I103" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I104" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I105" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I106" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I107" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I108" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I109" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I110" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I111" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I112" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L101"/>
   <sheetViews>
@@ -4988,7 +5820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55AB20B3-088A-4C48-9746-FAFDBAF6F80B}">
   <dimension ref="A1:L103"/>
   <sheetViews>
@@ -6141,7 +6973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B494BF-8FB3-4F10-BF9B-C1AB6CBBBD39}">
   <dimension ref="A1:L102"/>
   <sheetViews>

</xml_diff>

<commit_message>
PCB is basically done - components need parameters updated for BOM
</commit_message>
<xml_diff>
--- a/BOMs/sinking-clock-BOM-v3.xlsx
+++ b/BOMs/sinking-clock-BOM-v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E436CD14-C5C1-4224-B61B-CBD52D2EE7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2B506C-6FF1-417F-ADE8-DFF7F06755C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain PCB Assembly" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="333">
   <si>
     <t>Quantity</t>
   </si>
@@ -602,18 +602,9 @@
     <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/4149/10123800</t>
   </si>
   <si>
-    <t>battery</t>
-  </si>
-  <si>
     <t>battery connector</t>
   </si>
   <si>
-    <t xml:space="preserve">battery management IC stuff </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Debouncing ICs? </t>
-  </si>
-  <si>
     <t>150060RS75000</t>
   </si>
   <si>
@@ -912,9 +903,6 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/cui-devices/PJ-002BH-SMT-TR/404626</t>
-  </si>
-  <si>
-    <t>ferrite bead</t>
   </si>
   <si>
     <t>32.768 kHz crystal oscillator</t>
@@ -1599,9 +1587,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535EBE7C-EB1B-4F48-8827-B2C8DF8DD54E}">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1640,7 +1628,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>4</v>
@@ -1672,22 +1660,22 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="H3" s="11">
         <v>1</v>
@@ -1700,7 +1688,7 @@
         <v>3.31</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="M3" s="2">
         <f>SUM(J3:J113)</f>
@@ -1709,16 +1697,16 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>12</v>
@@ -1731,97 +1719,97 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="J5" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="J6" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="J7" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>12</v>
@@ -1834,16 +1822,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>12</v>
@@ -1856,16 +1844,16 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>12</v>
@@ -1878,16 +1866,16 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>12</v>
@@ -1900,22 +1888,22 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H12" s="11">
         <v>1</v>
@@ -1928,15 +1916,15 @@
         <v>0.68</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="14">
@@ -1947,10 +1935,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>72</v>
@@ -1980,37 +1968,37 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="J15" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J16" s="14">
         <f t="shared" si="0"/>
@@ -2022,7 +2010,7 @@
         <v>109</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>110</v>
@@ -2052,31 +2040,31 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="J18" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C19" s="29">
         <v>603</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J19" s="14">
         <f t="shared" si="0"/>
@@ -2086,16 +2074,16 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J20" s="14">
         <f t="shared" si="0"/>
@@ -2116,9 +2104,6 @@
       <c r="M21" s="2"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>188</v>
-      </c>
       <c r="I22" s="14"/>
       <c r="J22" s="14">
         <f t="shared" si="0"/>
@@ -2127,9 +2112,6 @@
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>189</v>
-      </c>
       <c r="J23" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2137,9 +2119,6 @@
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>190</v>
-      </c>
       <c r="J24" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2147,9 +2126,6 @@
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>291</v>
-      </c>
       <c r="J25" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2179,19 +2155,19 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J29" s="14">
         <f t="shared" si="0"/>
@@ -2785,19 +2761,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>57</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G3" s="11">
         <v>56</v>
@@ -2810,7 +2786,7 @@
         <v>7.9519999999999991</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="L3" s="2">
         <f>SUM(I3:I111)</f>
@@ -2819,19 +2795,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>57</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G4" s="11">
         <v>2</v>
@@ -2844,24 +2820,24 @@
         <v>0.4</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G5" s="11">
         <v>1</v>
@@ -2874,24 +2850,24 @@
         <v>0.32</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
         <v>212</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>215</v>
       </c>
       <c r="G6" s="11">
         <v>4</v>
@@ -2904,24 +2880,24 @@
         <v>1.88</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G7" s="11">
         <v>4</v>
@@ -2934,24 +2910,24 @@
         <v>0.4</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
         <v>253</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>256</v>
       </c>
       <c r="G8" s="11">
         <v>1</v>
@@ -2964,24 +2940,24 @@
         <v>0.68</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G9" s="11">
         <v>1</v>
@@ -2994,24 +2970,24 @@
         <v>0.37</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G10" s="11">
         <v>23</v>
@@ -3024,25 +3000,25 @@
         <v>4.4160000000000004</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G11" s="11">
         <v>3</v>
@@ -3055,24 +3031,24 @@
         <v>0.36</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>233</v>
-      </c>
       <c r="D12" s="11" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G12" s="11">
         <v>4</v>
@@ -3085,24 +3061,24 @@
         <v>0.4</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G13" s="11">
         <v>5</v>
@@ -3115,24 +3091,24 @@
         <v>0.5</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G14" s="11">
         <v>12</v>
@@ -3145,24 +3121,24 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>244</v>
-      </c>
       <c r="E15" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G15" s="11">
         <v>11</v>
@@ -3175,24 +3151,24 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G16" s="11">
         <v>2</v>
@@ -3205,24 +3181,24 @@
         <v>0.2</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G17" s="11">
         <v>9</v>
@@ -3235,7 +3211,7 @@
         <v>1.44</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
@@ -3828,9 +3804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7A9FC6-1251-4D6C-A8F0-29659EBD6918}">
   <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3896,19 +3872,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G3" s="11">
         <v>1</v>
@@ -3921,7 +3897,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="L3" s="2">
         <f>SUM(I3:I113)</f>
@@ -4109,16 +4085,16 @@
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I29" s="14">
         <f t="shared" si="0"/>
@@ -6979,7 +6955,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7045,22 +7021,22 @@
     </row>
     <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>57</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G3" s="20">
         <v>168</v>
@@ -7073,7 +7049,7 @@
         <v>23.855999999999998</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="L3" s="2">
         <f>SUM(I3:I101)</f>
@@ -7082,19 +7058,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>57</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G4" s="20">
         <v>6</v>
@@ -7107,24 +7083,24 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G5" s="20">
         <v>3</v>
@@ -7137,24 +7113,24 @@
         <v>0.96</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>212</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>215</v>
       </c>
       <c r="G6" s="20">
         <v>12</v>
@@ -7167,24 +7143,24 @@
         <v>5.64</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G7" s="20">
         <v>12</v>
@@ -7197,25 +7173,25 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>253</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>255</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>256</v>
       </c>
       <c r="G8" s="20">
         <v>3</v>
@@ -7228,24 +7204,24 @@
         <v>2.04</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G9" s="20">
         <v>3</v>
@@ -7258,24 +7234,24 @@
         <v>1.1099999999999999</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G10" s="20">
         <v>69</v>
@@ -7288,24 +7264,24 @@
         <v>13.248000000000001</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G11" s="20">
         <v>9</v>
@@ -7318,24 +7294,24 @@
         <v>1.08</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>233</v>
-      </c>
       <c r="D12" s="20" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G12" s="20">
         <v>12</v>
@@ -7348,24 +7324,24 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G13" s="20">
         <v>15</v>
@@ -7378,24 +7354,24 @@
         <v>1.5</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G14" s="20">
         <v>36</v>
@@ -7408,24 +7384,24 @@
         <v>3.6</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" s="19" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C15" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>244</v>
-      </c>
       <c r="E15" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G15" s="20">
         <v>33</v>
@@ -7438,24 +7414,24 @@
         <v>3.3000000000000003</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G16" s="20">
         <v>4</v>
@@ -7468,24 +7444,24 @@
         <v>0.4</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="19" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G17" s="20">
         <v>27</v>
@@ -7498,24 +7474,24 @@
         <v>4.32</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G18" s="11">
         <v>1</v>
@@ -7528,24 +7504,24 @@
         <v>22.16</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
         <v>263</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" t="s">
-        <v>266</v>
       </c>
       <c r="G19" s="11">
         <v>1</v>
@@ -7558,24 +7534,24 @@
         <v>42.86</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>83</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G20" s="11">
         <v>1</v>
@@ -7588,21 +7564,21 @@
         <v>20.95</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G21" s="11">
         <v>2</v>
@@ -7615,21 +7591,21 @@
         <v>0.42</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F22" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G22" s="11">
         <v>2</v>
@@ -7642,21 +7618,21 @@
         <v>0.86</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F23" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G23" s="11">
         <v>2</v>
@@ -7669,21 +7645,21 @@
         <v>0.86</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F24" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G24" s="11">
         <v>2</v>
@@ -7696,7 +7672,7 @@
         <v>0.92</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Altium BOM is up-to-date
</commit_message>
<xml_diff>
--- a/BOMs/sinking-clock-BOM-v3.xlsx
+++ b/BOMs/sinking-clock-BOM-v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2B506C-6FF1-417F-ADE8-DFF7F06755C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9ABAC18-5E9C-46CA-B3F3-D6F83D614A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="333">
   <si>
     <t>Quantity</t>
   </si>
@@ -1587,9 +1587,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535EBE7C-EB1B-4F48-8827-B2C8DF8DD54E}">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1778,25 +1778,8 @@
       <c r="C7" s="30" t="s">
         <v>295</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="J7" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>228</v>
-      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -2684,10 +2667,9 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K14" r:id="rId1" xr:uid="{206B78D0-3E11-49C8-918E-265464AE26FD}"/>
-    <hyperlink ref="K7" r:id="rId2" xr:uid="{6C5F0919-5E89-4DE3-A40D-FFBA722F20C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6954,8 +6936,8 @@
   <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7577,6 +7559,9 @@
       <c r="D21" s="11" t="s">
         <v>270</v>
       </c>
+      <c r="E21" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F21" t="s">
         <v>271</v>
       </c>
@@ -7604,6 +7589,9 @@
       <c r="D22" s="11" t="s">
         <v>275</v>
       </c>
+      <c r="E22" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F22" t="s">
         <v>276</v>
       </c>
@@ -7631,6 +7619,9 @@
       <c r="D23" s="11" t="s">
         <v>279</v>
       </c>
+      <c r="E23" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="F23" t="s">
         <v>280</v>
       </c>
@@ -7657,6 +7648,9 @@
       </c>
       <c r="D24" s="11" t="s">
         <v>283</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="F24" t="s">
         <v>284</v>

</xml_diff>

<commit_message>
BOM update with non-inverted polarity cable, add I2C to new pinout
</commit_message>
<xml_diff>
--- a/BOMs/sinking-clock-BOM-v3.xlsx
+++ b/BOMs/sinking-clock-BOM-v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sinking-clock\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5BB7F2-B669-420A-8E0C-28F62A9ABF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFE9EE5-132A-44E2-96B7-B156BF092504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brain PCB Assembly" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="335">
   <si>
     <t>Quantity</t>
   </si>
@@ -1038,6 +1038,12 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/nte-electronics-inc/57-PRP2/11644414</t>
+  </si>
+  <si>
+    <t>(???)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Fancasee-Extension-Wireless-Security-Surveillance/dp/B081TX6HB6/ref=sr_1_4</t>
   </si>
 </sst>
 </file>
@@ -1587,9 +1593,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535EBE7C-EB1B-4F48-8827-B2C8DF8DD54E}">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3786,9 +3792,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7A9FC6-1251-4D6C-A8F0-29659EBD6918}">
   <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3853,6 +3859,9 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="B3" t="s">
         <v>328</v>
       </c>
@@ -3891,7 +3900,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I5" s="14">

</xml_diff>